<commit_message>
updated naming and tagging excel typo
</commit_message>
<xml_diff>
--- a/ready/naming-and-tagging-conventions-tracking-template.xlsx
+++ b/ready/naming-and-tagging-conventions-tracking-template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDA9F84-7642-4467-AF44-48F4186AA6AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973BC622-71B7-47E8-9BAD-EBC57E0328F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27510" windowHeight="16440" xr2:uid="{210B74E1-E46B-4D63-B43A-5415A9E8F7DF}"/>
+    <workbookView xWindow="18540" yWindow="-21780" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{210B74E1-E46B-4D63-B43A-5415A9E8F7DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro and components" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="294">
   <si>
     <t>Microsoft Cloud Adoption Framework for Azure</t>
   </si>
@@ -1049,6 +1049,9 @@
   </si>
   <si>
     <t>Adoption Readiness: Naming and Tagging Conventions &lt;DRAFT&gt;</t>
+  </si>
+  <si>
+    <t>Naming conventions</t>
   </si>
 </sst>
 </file>
@@ -1277,9 +1280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1317,7 +1320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1423,7 +1426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1565,7 +1568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1575,33 +1578,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D934DE8B-7D3C-4126-9C22-7D22430A904E}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="17.149999999999999" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" style="2" customWidth="1"/>
-    <col min="2" max="7" width="35.140625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="36.53515625" style="2" customWidth="1"/>
+    <col min="2" max="7" width="35.15234375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="23.15" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="28.3" x14ac:dyDescent="0.8">
       <c r="A2" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.65">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>158</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>159</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="17" t="s">
         <v>5</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="85.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="87.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="18" t="s">
         <v>8</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="71.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="58.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="18" t="s">
         <v>10</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="29.15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="20" t="s">
         <v>12</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="42.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="29.15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="18" t="s">
         <v>14</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="29.15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -1699,7 +1702,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="20" t="s">
         <v>27</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="20" t="s">
         <v>29</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="20" t="s">
         <v>31</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="20" t="s">
         <v>33</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="20" t="s">
         <v>35</v>
       </c>
@@ -1755,7 +1758,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="20" t="s">
         <v>37</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="20" t="s">
         <v>39</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="20" t="s">
         <v>41</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="20" t="s">
         <v>43</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="20" t="s">
         <v>45</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="20" t="s">
         <v>47</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="20" t="s">
         <v>49</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="20" t="s">
         <v>51</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="20" t="s">
         <v>53</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="20" t="s">
         <v>55</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="20" t="s">
         <v>57</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="20" t="s">
         <v>59</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="20" t="s">
         <v>61</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="20" t="s">
         <v>63</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="20" t="s">
         <v>65</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="20" t="s">
         <v>67</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="20" t="s">
         <v>69</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="20" t="s">
         <v>71</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="20" t="s">
         <v>73</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="20" t="s">
         <v>75</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="20" t="s">
         <v>77</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="20" t="s">
         <v>79</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="20" t="s">
         <v>81</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="20" t="s">
         <v>83</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="20" t="s">
         <v>85</v>
       </c>
@@ -1955,7 +1958,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="20" t="s">
         <v>87</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="20" t="s">
         <v>89</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="20" t="s">
         <v>91</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="20" t="s">
         <v>93</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="20" t="s">
         <v>95</v>
       </c>
@@ -1995,7 +1998,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="20" t="s">
         <v>97</v>
       </c>
@@ -2003,7 +2006,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="20" t="s">
         <v>99</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="20" t="s">
         <v>101</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="20" t="s">
         <v>103</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="20" t="s">
         <v>105</v>
       </c>
@@ -2045,27 +2048,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76278524-D3B2-4667-AD71-4E312091F8FD}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="17.149999999999999" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="52.85546875" style="2" customWidth="1"/>
-    <col min="5" max="7" width="28.42578125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="37.3828125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.15234375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="65.15234375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="52.84375" style="2" customWidth="1"/>
+    <col min="5" max="7" width="28.3828125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
-        <v>107</v>
+        <v>293</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
@@ -2073,12 +2074,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11" t="s">
         <v>165</v>
       </c>
@@ -2092,7 +2093,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
         <v>168</v>
       </c>
@@ -2106,13 +2107,13 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
         <v>173</v>
       </c>
@@ -2120,7 +2121,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11" t="s">
         <v>165</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="12" t="s">
         <v>174</v>
       </c>
@@ -2148,13 +2149,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
         <v>177</v>
       </c>
@@ -2162,7 +2163,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11" t="s">
         <v>165</v>
       </c>
@@ -2176,7 +2177,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12" t="s">
         <v>178</v>
       </c>
@@ -2190,7 +2191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="12" t="s">
         <v>181</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="12" t="s">
         <v>184</v>
       </c>
@@ -2218,7 +2219,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
         <v>188</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
         <v>191</v>
       </c>
@@ -2246,7 +2247,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="12" t="s">
         <v>35</v>
       </c>
@@ -2260,7 +2261,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
         <v>37</v>
       </c>
@@ -2274,7 +2275,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
         <v>43</v>
       </c>
@@ -2288,12 +2289,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="17" t="s">
         <v>165</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="20" t="s">
         <v>205</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="20" t="s">
         <v>208</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="20" t="s">
         <v>212</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="20" t="s">
         <v>215</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="20" t="s">
         <v>47</v>
       </c>
@@ -2377,12 +2378,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="17" t="s">
         <v>165</v>
       </c>
@@ -2396,7 +2397,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="20" t="s">
         <v>221</v>
       </c>
@@ -2410,7 +2411,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="20" t="s">
         <v>224</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="20" t="s">
         <v>57</v>
       </c>
@@ -2438,12 +2439,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="17" t="s">
         <v>165</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="20" t="s">
         <v>49</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="20" t="s">
         <v>51</v>
       </c>
@@ -2485,12 +2486,12 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="9" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="17" t="s">
         <v>165</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="20" t="s">
         <v>59</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="20" t="s">
         <v>61</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="20" t="s">
         <v>63</v>
       </c>
@@ -2546,7 +2547,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="20" t="s">
         <v>65</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="20" t="s">
         <v>67</v>
       </c>
@@ -2574,7 +2575,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="20" t="s">
         <v>69</v>
       </c>
@@ -2588,12 +2589,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="17" t="s">
         <v>165</v>
       </c>
@@ -2607,7 +2608,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="20" t="s">
         <v>247</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="20" t="s">
         <v>250</v>
       </c>
@@ -2635,7 +2636,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="20" t="s">
         <v>73</v>
       </c>
@@ -2649,12 +2650,12 @@
         <v>254</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="9" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="17" t="s">
         <v>165</v>
       </c>
@@ -2668,7 +2669,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="20" t="s">
         <v>75</v>
       </c>
@@ -2682,7 +2683,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="20" t="s">
         <v>77</v>
       </c>
@@ -2696,7 +2697,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="20" t="s">
         <v>79</v>
       </c>
@@ -2710,12 +2711,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="9" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="17" t="s">
         <v>165</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="20" t="s">
         <v>263</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="20" t="s">
         <v>81</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="20" t="s">
         <v>83</v>
       </c>
@@ -2771,7 +2772,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="20" t="s">
         <v>85</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="20" t="s">
         <v>87</v>
       </c>
@@ -2799,7 +2800,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="20" t="s">
         <v>89</v>
       </c>
@@ -2813,7 +2814,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="20" t="s">
         <v>91</v>
       </c>
@@ -2827,7 +2828,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="20" t="s">
         <v>93</v>
       </c>
@@ -2841,12 +2842,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="9" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="17" t="s">
         <v>165</v>
       </c>
@@ -2860,7 +2861,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="20" t="s">
         <v>281</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="20" t="s">
         <v>101</v>
       </c>
@@ -2888,7 +2889,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="20" t="s">
         <v>99</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="20" t="s">
         <v>288</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="20" t="s">
         <v>105</v>
       </c>
@@ -2944,20 +2945,20 @@
       <selection activeCell="B8" sqref="A4:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="17.149999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="27.3828125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="45.69140625" style="7" customWidth="1"/>
     <col min="3" max="7" width="33" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="8" max="16384" width="9.15234375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>109</v>
       </c>
@@ -2982,7 +2983,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>112</v>
       </c>
@@ -2999,7 +3000,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
         <v>116</v>
       </c>
@@ -3016,7 +3017,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>120</v>
       </c>
@@ -3033,7 +3034,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="85.75" x14ac:dyDescent="0.4">
       <c r="A8" s="15" t="s">
         <v>124</v>
       </c>
@@ -3050,7 +3051,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
         <v>128</v>
       </c>
@@ -3067,7 +3068,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A10" s="15" t="s">
         <v>132</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A11" s="15" t="s">
         <v>136</v>
       </c>
@@ -3101,7 +3102,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A12" s="15" t="s">
         <v>140</v>
       </c>
@@ -3118,7 +3119,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="15" t="s">
         <v>144</v>
       </c>
@@ -3135,7 +3136,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A14" s="15" t="s">
         <v>147</v>
       </c>
@@ -3152,7 +3153,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>150</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="34.299999999999997" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
         <v>154</v>
       </c>
@@ -3190,4 +3191,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>